<commit_message>
Add notes on Frequency distributions
</commit_message>
<xml_diff>
--- a/Basic Analysis/Conditional Aggregations/Conditional Aggregations Quiz Workbook.xlsx
+++ b/Basic Analysis/Conditional Aggregations/Conditional Aggregations Quiz Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Friedturnip\Desktop\Data Foundations BUILD\Aggregating Data\Conditional formulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Basic Analysis\Conditional Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7618740F-DD65-4D99-B40F-7CCF244C96DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8AF78B-F15A-4FE9-9AC8-18A8E92C067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="630" windowWidth="24660" windowHeight="14895" tabRatio="515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="600" windowWidth="29850" windowHeight="14805" tabRatio="515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="salaries" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">salaries!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -256,8 +246,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -728,7 +718,7 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -771,20 +761,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1146,20 +1133,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" customWidth="1"/>
@@ -1167,661 +1154,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="10"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>89256</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="4">
+        <f>COUNTIF($C:$C,"Cert4")</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>86405</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="4">
+        <f>COUNTIF($C:$C,"Advanced Diploma")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>132057</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="4">
+        <f>COUNTIF(D:D,"Data")</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>68754</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="4">
+        <f>COUNTIFS(E:E,"Data Scientist",C:C,"Advanced Diploma")</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>64215</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="4">
+        <f>COUNTIF(B2:B20,"")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>48153</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>63152</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>92182</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>81306</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="4">
+        <f>SUMIFS($F:$F,D:D,"Data")</f>
+        <v>936311</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>62156</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="4">
+        <f>SUMIFS(F:F,C:C,"Masters Degree")</f>
+        <v>466835</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>63152</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="4">
+        <f>SUMIFS(F:F,E:E,"Research Associate")</f>
+        <v>190519</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66604</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="4">
+        <f>SUMIFS(F:F,D:D,"Data",C:C,"Advanced Diploma")</f>
+        <v>349149</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>72561</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="4">
+        <f>SUMIFS(F:F,E:E,"Data Scientist",C:C,"Bachelor Degree")</f>
+        <v>103465</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>121374</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>103465</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>105513</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>114048</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>115217</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>67903</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>